<commit_message>
Se termino etapa 1 de replicacion de template para Olimpia con archivos locales
</commit_message>
<xml_diff>
--- a/Template_HRC.xlsx
+++ b/Template_HRC.xlsx
@@ -60,6 +60,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -72,7 +73,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C18:I72"/>
+  <dimension ref="C2:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,257 +447,371 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Desglose de Pago</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>REFERENCIA DE PAGO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>PK003702815749</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CAMPOS NO EDITABLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SUPERTIENDAS Y DROGUERIAS OLIM</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TOTAL s/ BANCOS</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>1047007047</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>TOTAL s/ DETALLE</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1047007084.72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Codigo de Cliente</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10266237</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>DIFERENCIA</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>-37.71999996528029</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Referencia</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Método de Pago</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PK003702815749</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>8/11/25</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Transferencia</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>1047007047</v>
+      </c>
+    </row>
     <row r="18">
-      <c r="C18" s="2" t="inlineStr">
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>Tipo de Documento</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="D18" s="3" t="inlineStr">
         <is>
           <t>Referencia / Factura</t>
         </is>
       </c>
-      <c r="E18" s="3" t="inlineStr">
+      <c r="E18" s="4" t="inlineStr">
         <is>
           <t>Importe de factura</t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>Descuento</t>
         </is>
       </c>
-      <c r="G18" s="2" t="inlineStr">
+      <c r="G18" s="3" t="inlineStr">
         <is>
           <t>Motivo del descuento</t>
         </is>
       </c>
-      <c r="H18" s="3" t="inlineStr">
+      <c r="H18" s="4" t="inlineStr">
         <is>
           <t>Pago Neto</t>
         </is>
       </c>
-      <c r="I18" s="4" t="inlineStr">
+      <c r="I18" s="5" t="inlineStr">
         <is>
           <t>Comentarios</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="5" t="inlineStr">
+      <c r="C19" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D19" s="5" t="inlineStr">
+      <c r="D19" s="6" t="inlineStr">
         <is>
           <t>PMP1243434</t>
         </is>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="2" t="n">
         <v>165989699</v>
       </c>
-      <c r="F19" s="5" t="inlineStr"/>
-      <c r="G19" s="5" t="inlineStr"/>
-      <c r="H19" s="6" t="n">
+      <c r="F19" s="6" t="inlineStr"/>
+      <c r="G19" s="6" t="inlineStr"/>
+      <c r="H19" s="2" t="n">
         <v>165989699</v>
       </c>
       <c r="I19" s="7" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="C20" s="5" t="inlineStr">
+      <c r="C20" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
+      <c r="D20" s="6" t="inlineStr">
         <is>
           <t>PMP1243435</t>
         </is>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E20" s="2" t="n">
         <v>29856410</v>
       </c>
-      <c r="F20" s="5" t="inlineStr"/>
-      <c r="G20" s="5" t="inlineStr"/>
-      <c r="H20" s="6" t="n">
+      <c r="F20" s="6" t="inlineStr"/>
+      <c r="G20" s="6" t="inlineStr"/>
+      <c r="H20" s="2" t="n">
         <v>29856410</v>
       </c>
       <c r="I20" s="7" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="C21" s="5" t="inlineStr">
+      <c r="C21" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D21" s="5" t="inlineStr">
+      <c r="D21" s="6" t="inlineStr">
         <is>
           <t>PMP1243436</t>
         </is>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E21" s="2" t="n">
         <v>12528130</v>
       </c>
-      <c r="F21" s="5" t="inlineStr"/>
-      <c r="G21" s="5" t="inlineStr"/>
-      <c r="H21" s="6" t="n">
+      <c r="F21" s="6" t="inlineStr"/>
+      <c r="G21" s="6" t="inlineStr"/>
+      <c r="H21" s="2" t="n">
         <v>12528130</v>
       </c>
       <c r="I21" s="7" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="C22" s="5" t="inlineStr">
+      <c r="C22" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D22" s="5" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr">
         <is>
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E22" s="6" t="n">
+      <c r="E22" s="2" t="n">
         <v>83124</v>
       </c>
-      <c r="F22" s="5" t="inlineStr"/>
-      <c r="G22" s="5" t="inlineStr"/>
-      <c r="H22" s="6" t="n">
+      <c r="F22" s="6" t="inlineStr"/>
+      <c r="G22" s="6" t="inlineStr"/>
+      <c r="H22" s="2" t="n">
         <v>83124</v>
       </c>
       <c r="I22" s="7" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="C23" s="5" t="inlineStr">
+      <c r="C23" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D23" s="5" t="inlineStr">
+      <c r="D23" s="6" t="inlineStr">
         <is>
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="2" t="n">
         <v>53514044</v>
       </c>
-      <c r="F23" s="5" t="inlineStr"/>
-      <c r="G23" s="5" t="inlineStr"/>
-      <c r="H23" s="6" t="n">
+      <c r="F23" s="6" t="inlineStr"/>
+      <c r="G23" s="6" t="inlineStr"/>
+      <c r="H23" s="2" t="n">
         <v>53514044</v>
       </c>
       <c r="I23" s="7" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="C24" s="5" t="inlineStr">
+      <c r="C24" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D24" s="5" t="inlineStr">
+      <c r="D24" s="6" t="inlineStr">
         <is>
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E24" s="6" t="n">
+      <c r="E24" s="2" t="n">
         <v>757032037</v>
       </c>
-      <c r="F24" s="5" t="inlineStr"/>
-      <c r="G24" s="5" t="inlineStr"/>
-      <c r="H24" s="6" t="n">
+      <c r="F24" s="6" t="inlineStr"/>
+      <c r="G24" s="6" t="inlineStr"/>
+      <c r="H24" s="2" t="n">
         <v>757032037</v>
       </c>
       <c r="I24" s="7" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="C25" s="5" t="inlineStr">
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E25" s="6" t="n">
+      <c r="E25" s="2" t="n">
         <v>122759901</v>
       </c>
-      <c r="F25" s="5" t="inlineStr"/>
-      <c r="G25" s="5" t="inlineStr"/>
-      <c r="H25" s="6" t="n">
+      <c r="F25" s="6" t="inlineStr"/>
+      <c r="G25" s="6" t="inlineStr"/>
+      <c r="H25" s="2" t="n">
         <v>122759901</v>
       </c>
       <c r="I25" s="7" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="C26" s="5" t="inlineStr">
+      <c r="C26" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D26" s="5" t="inlineStr">
+      <c r="D26" s="6" t="inlineStr">
         <is>
           <t>PMP1243587</t>
         </is>
       </c>
-      <c r="E26" s="6" t="n">
+      <c r="E26" s="2" t="n">
         <v>132622525</v>
       </c>
-      <c r="F26" s="5" t="inlineStr"/>
-      <c r="G26" s="5" t="inlineStr"/>
-      <c r="H26" s="6" t="n">
+      <c r="F26" s="6" t="inlineStr"/>
+      <c r="G26" s="6" t="inlineStr"/>
+      <c r="H26" s="2" t="n">
         <v>132622525</v>
       </c>
       <c r="I26" s="7" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="C27" s="5" t="inlineStr">
+      <c r="C27" s="6" t="inlineStr">
         <is>
           <t>Factura</t>
         </is>
       </c>
-      <c r="D27" s="5" t="inlineStr">
+      <c r="D27" s="6" t="inlineStr">
         <is>
           <t>PMP1243639</t>
         </is>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="2" t="n">
         <v>343873745</v>
       </c>
-      <c r="F27" s="5" t="inlineStr"/>
-      <c r="G27" s="5" t="inlineStr"/>
-      <c r="H27" s="6" t="n">
+      <c r="F27" s="6" t="inlineStr"/>
+      <c r="G27" s="6" t="inlineStr"/>
+      <c r="H27" s="2" t="n">
         <v>343873745</v>
       </c>
       <c r="I27" s="7" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="C28" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D28" s="5" t="inlineStr">
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
         <is>
           <t>0085489002</t>
         </is>
       </c>
-      <c r="E28" s="6" t="n">
+      <c r="E28" s="2" t="n">
         <v>-106616</v>
       </c>
-      <c r="F28" s="5" t="inlineStr">
+      <c r="F28" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G28" s="5" t="inlineStr">
+      <c r="G28" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H28" s="6" t="n">
+      <c r="H28" s="2" t="n">
         <v>-106616</v>
       </c>
       <c r="I28" s="7" t="inlineStr">
@@ -707,30 +821,30 @@
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D29" s="5" t="inlineStr">
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
         <is>
           <t>0085489003</t>
         </is>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="2" t="n">
         <v>-280732</v>
       </c>
-      <c r="F29" s="5" t="inlineStr">
+      <c r="F29" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G29" s="5" t="inlineStr">
+      <c r="G29" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H29" s="6" t="n">
+      <c r="H29" s="2" t="n">
         <v>-280732</v>
       </c>
       <c r="I29" s="7" t="inlineStr">
@@ -740,30 +854,30 @@
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D30" s="5" t="inlineStr">
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
         <is>
           <t>0085489004</t>
         </is>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="2" t="n">
         <v>-852931</v>
       </c>
-      <c r="F30" s="5" t="inlineStr">
+      <c r="F30" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G30" s="5" t="inlineStr">
+      <c r="G30" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H30" s="6" t="n">
+      <c r="H30" s="2" t="n">
         <v>-852931</v>
       </c>
       <c r="I30" s="7" t="inlineStr">
@@ -773,30 +887,30 @@
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D31" s="5" t="inlineStr">
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
         <is>
           <t>0085489005</t>
         </is>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E31" s="2" t="n">
         <v>-1235221</v>
       </c>
-      <c r="F31" s="5" t="inlineStr">
+      <c r="F31" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G31" s="5" t="inlineStr">
+      <c r="G31" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H31" s="6" t="n">
+      <c r="H31" s="2" t="n">
         <v>-1235221</v>
       </c>
       <c r="I31" s="7" t="inlineStr">
@@ -806,30 +920,30 @@
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D32" s="5" t="inlineStr">
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D32" s="6" t="inlineStr">
         <is>
           <t>0085489006</t>
         </is>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="2" t="n">
         <v>-2772024</v>
       </c>
-      <c r="F32" s="5" t="inlineStr">
+      <c r="F32" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G32" s="5" t="inlineStr">
+      <c r="G32" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H32" s="6" t="n">
+      <c r="H32" s="2" t="n">
         <v>-2772024</v>
       </c>
       <c r="I32" s="7" t="inlineStr">
@@ -839,30 +953,30 @@
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D33" s="5" t="inlineStr">
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t>0085489007</t>
         </is>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="2" t="n">
         <v>-3198490</v>
       </c>
-      <c r="F33" s="5" t="inlineStr">
+      <c r="F33" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G33" s="5" t="inlineStr">
+      <c r="G33" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H33" s="2" t="n">
         <v>-3198490</v>
       </c>
       <c r="I33" s="7" t="inlineStr">
@@ -872,30 +986,30 @@
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D34" s="5" t="inlineStr">
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D34" s="6" t="inlineStr">
         <is>
           <t>0085489008</t>
         </is>
       </c>
-      <c r="E34" s="6" t="n">
+      <c r="E34" s="2" t="n">
         <v>-4472640</v>
       </c>
-      <c r="F34" s="5" t="inlineStr">
+      <c r="F34" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G34" s="5" t="inlineStr">
+      <c r="G34" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H34" s="6" t="n">
+      <c r="H34" s="2" t="n">
         <v>-4472640</v>
       </c>
       <c r="I34" s="7" t="inlineStr">
@@ -905,30 +1019,30 @@
       </c>
     </row>
     <row r="35">
-      <c r="C35" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D35" s="5" t="inlineStr">
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="inlineStr">
         <is>
           <t>0085489009</t>
         </is>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="2" t="n">
         <v>-4895525</v>
       </c>
-      <c r="F35" s="5" t="inlineStr">
+      <c r="F35" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G35" s="5" t="inlineStr">
+      <c r="G35" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H35" s="6" t="n">
+      <c r="H35" s="2" t="n">
         <v>-4895525</v>
       </c>
       <c r="I35" s="7" t="inlineStr">
@@ -938,30 +1052,30 @@
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D36" s="5" t="inlineStr">
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="inlineStr">
         <is>
           <t>0085489010</t>
         </is>
       </c>
-      <c r="E36" s="6" t="n">
+      <c r="E36" s="2" t="n">
         <v>-6266272</v>
       </c>
-      <c r="F36" s="5" t="inlineStr">
+      <c r="F36" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G36" s="5" t="inlineStr">
+      <c r="G36" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H36" s="6" t="n">
+      <c r="H36" s="2" t="n">
         <v>-6266272</v>
       </c>
       <c r="I36" s="7" t="inlineStr">
@@ -971,30 +1085,30 @@
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D37" s="5" t="inlineStr">
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
         <is>
           <t>0085489011</t>
         </is>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E37" s="2" t="n">
         <v>-7156225</v>
       </c>
-      <c r="F37" s="5" t="inlineStr">
+      <c r="F37" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G37" s="5" t="inlineStr">
+      <c r="G37" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H37" s="6" t="n">
+      <c r="H37" s="2" t="n">
         <v>-7156225</v>
       </c>
       <c r="I37" s="7" t="inlineStr">
@@ -1004,30 +1118,30 @@
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D38" s="5" t="inlineStr">
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D38" s="6" t="inlineStr">
         <is>
           <t>0085489012</t>
         </is>
       </c>
-      <c r="E38" s="6" t="n">
+      <c r="E38" s="2" t="n">
         <v>-7343319</v>
       </c>
-      <c r="F38" s="5" t="inlineStr">
+      <c r="F38" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G38" s="5" t="inlineStr">
+      <c r="G38" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H38" s="6" t="n">
+      <c r="H38" s="2" t="n">
         <v>-7343319</v>
       </c>
       <c r="I38" s="7" t="inlineStr">
@@ -1037,30 +1151,30 @@
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D39" s="5" t="inlineStr">
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="inlineStr">
         <is>
           <t>0085489013</t>
         </is>
       </c>
-      <c r="E39" s="6" t="n">
+      <c r="E39" s="2" t="n">
         <v>-16267041</v>
       </c>
-      <c r="F39" s="5" t="inlineStr">
+      <c r="F39" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G39" s="5" t="inlineStr">
+      <c r="G39" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H39" s="6" t="n">
+      <c r="H39" s="2" t="n">
         <v>-16267041</v>
       </c>
       <c r="I39" s="7" t="inlineStr">
@@ -1070,30 +1184,30 @@
       </c>
     </row>
     <row r="40">
-      <c r="C40" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D40" s="5" t="inlineStr">
+      <c r="C40" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="inlineStr">
         <is>
           <t>0085489014</t>
         </is>
       </c>
-      <c r="E40" s="6" t="n">
+      <c r="E40" s="2" t="n">
         <v>-19679618</v>
       </c>
-      <c r="F40" s="5" t="inlineStr">
+      <c r="F40" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G40" s="5" t="inlineStr">
+      <c r="G40" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H40" s="6" t="n">
+      <c r="H40" s="2" t="n">
         <v>-19679618</v>
       </c>
       <c r="I40" s="7" t="inlineStr">
@@ -1103,30 +1217,30 @@
       </c>
     </row>
     <row r="41">
-      <c r="C41" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D41" s="5" t="inlineStr">
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D41" s="6" t="inlineStr">
         <is>
           <t>0085489015</t>
         </is>
       </c>
-      <c r="E41" s="6" t="n">
+      <c r="E41" s="2" t="n">
         <v>-22519415</v>
       </c>
-      <c r="F41" s="5" t="inlineStr">
+      <c r="F41" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G41" s="5" t="inlineStr">
+      <c r="G41" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H41" s="6" t="n">
+      <c r="H41" s="2" t="n">
         <v>-22519415</v>
       </c>
       <c r="I41" s="7" t="inlineStr">
@@ -1136,30 +1250,30 @@
       </c>
     </row>
     <row r="42">
-      <c r="C42" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D42" s="5" t="inlineStr">
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D42" s="6" t="inlineStr">
         <is>
           <t>0085489016</t>
         </is>
       </c>
-      <c r="E42" s="6" t="n">
+      <c r="E42" s="2" t="n">
         <v>-24608350</v>
       </c>
-      <c r="F42" s="5" t="inlineStr">
+      <c r="F42" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G42" s="5" t="inlineStr">
+      <c r="G42" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H42" s="6" t="n">
+      <c r="H42" s="2" t="n">
         <v>-24608350</v>
       </c>
       <c r="I42" s="7" t="inlineStr">
@@ -1169,30 +1283,30 @@
       </c>
     </row>
     <row r="43">
-      <c r="C43" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D43" s="5" t="inlineStr">
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D43" s="6" t="inlineStr">
         <is>
           <t>0085489017</t>
         </is>
       </c>
-      <c r="E43" s="6" t="n">
+      <c r="E43" s="2" t="n">
         <v>-63642284</v>
       </c>
-      <c r="F43" s="5" t="inlineStr">
+      <c r="F43" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G43" s="5" t="inlineStr">
+      <c r="G43" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H43" s="6" t="n">
+      <c r="H43" s="2" t="n">
         <v>-63642284</v>
       </c>
       <c r="I43" s="7" t="inlineStr">
@@ -1202,30 +1316,30 @@
       </c>
     </row>
     <row r="44">
-      <c r="C44" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D44" s="5" t="inlineStr">
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D44" s="6" t="inlineStr">
         <is>
           <t>0085489018</t>
         </is>
       </c>
-      <c r="E44" s="6" t="n">
+      <c r="E44" s="2" t="n">
         <v>-77643586</v>
       </c>
-      <c r="F44" s="5" t="inlineStr">
+      <c r="F44" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G44" s="5" t="inlineStr">
+      <c r="G44" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H44" s="6" t="n">
+      <c r="H44" s="2" t="n">
         <v>-77643586</v>
       </c>
       <c r="I44" s="7" t="inlineStr">
@@ -1235,30 +1349,30 @@
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D45" s="5" t="inlineStr">
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
         <is>
           <t>0085489642</t>
         </is>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="2" t="n">
         <v>-38727613</v>
       </c>
-      <c r="F45" s="5" t="inlineStr">
+      <c r="F45" s="6" t="inlineStr">
         <is>
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="G45" s="5" t="inlineStr">
+      <c r="G45" s="6" t="inlineStr">
         <is>
           <t>987</t>
         </is>
       </c>
-      <c r="H45" s="6" t="n">
+      <c r="H45" s="2" t="n">
         <v>-38727613</v>
       </c>
       <c r="I45" s="7" t="inlineStr">
@@ -1268,30 +1382,30 @@
       </c>
     </row>
     <row r="46">
-      <c r="C46" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D46" s="5" t="inlineStr">
+      <c r="C46" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D46" s="6" t="inlineStr">
         <is>
           <t>4631066394</t>
         </is>
       </c>
-      <c r="E46" s="6" t="n">
+      <c r="E46" s="2" t="n">
         <v>-35833</v>
       </c>
-      <c r="F46" s="5" t="inlineStr">
+      <c r="F46" s="6" t="inlineStr">
         <is>
           <t>AVERIA</t>
         </is>
       </c>
-      <c r="G46" s="5" t="inlineStr">
+      <c r="G46" s="6" t="inlineStr">
         <is>
           <t>522</t>
         </is>
       </c>
-      <c r="H46" s="6" t="n">
+      <c r="H46" s="2" t="n">
         <v>-35833</v>
       </c>
       <c r="I46" s="7" t="inlineStr">
@@ -1301,30 +1415,30 @@
       </c>
     </row>
     <row r="47">
-      <c r="C47" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D47" s="5" t="inlineStr">
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
         <is>
           <t>4633043274</t>
         </is>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="2" t="n">
         <v>-107500</v>
       </c>
-      <c r="F47" s="5" t="inlineStr">
+      <c r="F47" s="6" t="inlineStr">
         <is>
           <t>AVERIA</t>
         </is>
       </c>
-      <c r="G47" s="5" t="inlineStr">
+      <c r="G47" s="6" t="inlineStr">
         <is>
           <t>522</t>
         </is>
       </c>
-      <c r="H47" s="6" t="n">
+      <c r="H47" s="2" t="n">
         <v>-107500</v>
       </c>
       <c r="I47" s="7" t="inlineStr">
@@ -1334,30 +1448,30 @@
       </c>
     </row>
     <row r="48">
-      <c r="C48" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D48" s="5" t="inlineStr">
+      <c r="C48" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="inlineStr">
         <is>
           <t>4633141222</t>
         </is>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="2" t="n">
         <v>-31860</v>
       </c>
-      <c r="F48" s="5" t="inlineStr">
+      <c r="F48" s="6" t="inlineStr">
         <is>
           <t>AVERIA</t>
         </is>
       </c>
-      <c r="G48" s="5" t="inlineStr">
+      <c r="G48" s="6" t="inlineStr">
         <is>
           <t>522</t>
         </is>
       </c>
-      <c r="H48" s="6" t="n">
+      <c r="H48" s="2" t="n">
         <v>-31860</v>
       </c>
       <c r="I48" s="7" t="inlineStr">
@@ -1367,30 +1481,30 @@
       </c>
     </row>
     <row r="49">
-      <c r="C49" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D49" s="5" t="inlineStr">
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
         <is>
           <t>4633373549</t>
         </is>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="2" t="n">
         <v>-29575</v>
       </c>
-      <c r="F49" s="5" t="inlineStr">
+      <c r="F49" s="6" t="inlineStr">
         <is>
           <t>AVERIA</t>
         </is>
       </c>
-      <c r="G49" s="5" t="inlineStr">
+      <c r="G49" s="6" t="inlineStr">
         <is>
           <t>522</t>
         </is>
       </c>
-      <c r="H49" s="6" t="n">
+      <c r="H49" s="2" t="n">
         <v>-29575</v>
       </c>
       <c r="I49" s="7" t="inlineStr">
@@ -1400,30 +1514,30 @@
       </c>
     </row>
     <row r="50">
-      <c r="C50" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D50" s="5" t="inlineStr">
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
         <is>
           <t>9801649295</t>
         </is>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="2" t="n">
         <v>-817632</v>
       </c>
-      <c r="F50" s="5" t="inlineStr">
+      <c r="F50" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G50" s="5" t="inlineStr">
+      <c r="G50" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H50" s="6" t="n">
+      <c r="H50" s="2" t="n">
         <v>-817632</v>
       </c>
       <c r="I50" s="7" t="inlineStr">
@@ -1433,30 +1547,30 @@
       </c>
     </row>
     <row r="51">
-      <c r="C51" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D51" s="5" t="inlineStr">
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
         <is>
           <t>9801649296</t>
         </is>
       </c>
-      <c r="E51" s="6" t="n">
+      <c r="E51" s="2" t="n">
         <v>-817632</v>
       </c>
-      <c r="F51" s="5" t="inlineStr">
+      <c r="F51" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G51" s="5" t="inlineStr">
+      <c r="G51" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H51" s="6" t="n">
+      <c r="H51" s="2" t="n">
         <v>-817632</v>
       </c>
       <c r="I51" s="7" t="inlineStr">
@@ -1466,30 +1580,30 @@
       </c>
     </row>
     <row r="52">
-      <c r="C52" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D52" s="5" t="inlineStr">
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
         <is>
           <t>9801649297</t>
         </is>
       </c>
-      <c r="E52" s="6" t="n">
+      <c r="E52" s="2" t="n">
         <v>-3353617</v>
       </c>
-      <c r="F52" s="5" t="inlineStr">
+      <c r="F52" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G52" s="5" t="inlineStr">
+      <c r="G52" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H52" s="6" t="n">
+      <c r="H52" s="2" t="n">
         <v>-3353617</v>
       </c>
       <c r="I52" s="7" t="inlineStr">
@@ -1499,30 +1613,30 @@
       </c>
     </row>
     <row r="53">
-      <c r="C53" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D53" s="5" t="inlineStr">
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
         <is>
           <t>9801649298</t>
         </is>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="2" t="n">
         <v>-13687887</v>
       </c>
-      <c r="F53" s="5" t="inlineStr">
+      <c r="F53" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G53" s="5" t="inlineStr">
+      <c r="G53" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H53" s="6" t="n">
+      <c r="H53" s="2" t="n">
         <v>-13687887</v>
       </c>
       <c r="I53" s="7" t="inlineStr">
@@ -1532,30 +1646,30 @@
       </c>
     </row>
     <row r="54">
-      <c r="C54" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D54" s="5" t="inlineStr">
+      <c r="C54" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D54" s="6" t="inlineStr">
         <is>
           <t>9801649299</t>
         </is>
       </c>
-      <c r="E54" s="6" t="n">
+      <c r="E54" s="2" t="n">
         <v>-14589753</v>
       </c>
-      <c r="F54" s="5" t="inlineStr">
+      <c r="F54" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G54" s="5" t="inlineStr">
+      <c r="G54" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H54" s="6" t="n">
+      <c r="H54" s="2" t="n">
         <v>-14589753</v>
       </c>
       <c r="I54" s="7" t="inlineStr">
@@ -1565,30 +1679,30 @@
       </c>
     </row>
     <row r="55">
-      <c r="C55" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D55" s="5" t="inlineStr">
+      <c r="C55" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
         <is>
           <t>9801649300</t>
         </is>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="2" t="n">
         <v>-16674003</v>
       </c>
-      <c r="F55" s="5" t="inlineStr">
+      <c r="F55" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G55" s="5" t="inlineStr">
+      <c r="G55" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H55" s="6" t="n">
+      <c r="H55" s="2" t="n">
         <v>-16674003</v>
       </c>
       <c r="I55" s="7" t="inlineStr">
@@ -1598,30 +1712,30 @@
       </c>
     </row>
     <row r="56">
-      <c r="C56" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D56" s="5" t="inlineStr">
+      <c r="C56" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D56" s="6" t="inlineStr">
         <is>
           <t>9801649301</t>
         </is>
       </c>
-      <c r="E56" s="6" t="n">
+      <c r="E56" s="2" t="n">
         <v>-19800379</v>
       </c>
-      <c r="F56" s="5" t="inlineStr">
+      <c r="F56" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G56" s="5" t="inlineStr">
+      <c r="G56" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H56" s="6" t="n">
+      <c r="H56" s="2" t="n">
         <v>-19800379</v>
       </c>
       <c r="I56" s="7" t="inlineStr">
@@ -1631,30 +1745,30 @@
       </c>
     </row>
     <row r="57">
-      <c r="C57" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D57" s="5" t="inlineStr">
+      <c r="C57" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
         <is>
           <t>9801649302</t>
         </is>
       </c>
-      <c r="E57" s="6" t="n">
+      <c r="E57" s="2" t="n">
         <v>-21786554</v>
       </c>
-      <c r="F57" s="5" t="inlineStr">
+      <c r="F57" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G57" s="5" t="inlineStr">
+      <c r="G57" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H57" s="6" t="n">
+      <c r="H57" s="2" t="n">
         <v>-21786554</v>
       </c>
       <c r="I57" s="7" t="inlineStr">
@@ -1664,30 +1778,30 @@
       </c>
     </row>
     <row r="58">
-      <c r="C58" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D58" s="5" t="inlineStr">
+      <c r="C58" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D58" s="6" t="inlineStr">
         <is>
           <t>9801649303</t>
         </is>
       </c>
-      <c r="E58" s="6" t="n">
+      <c r="E58" s="2" t="n">
         <v>-47451687</v>
       </c>
-      <c r="F58" s="5" t="inlineStr">
+      <c r="F58" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G58" s="5" t="inlineStr">
+      <c r="G58" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H58" s="6" t="n">
+      <c r="H58" s="2" t="n">
         <v>-47451687</v>
       </c>
       <c r="I58" s="7" t="inlineStr">
@@ -1697,30 +1811,30 @@
       </c>
     </row>
     <row r="59">
-      <c r="C59" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D59" s="5" t="inlineStr">
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
         <is>
           <t>9801649304</t>
         </is>
       </c>
-      <c r="E59" s="6" t="n">
+      <c r="E59" s="2" t="n">
         <v>-54866013</v>
       </c>
-      <c r="F59" s="5" t="inlineStr">
+      <c r="F59" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G59" s="5" t="inlineStr">
+      <c r="G59" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H59" s="6" t="n">
+      <c r="H59" s="2" t="n">
         <v>-54866013</v>
       </c>
       <c r="I59" s="7" t="inlineStr">
@@ -1730,30 +1844,30 @@
       </c>
     </row>
     <row r="60">
-      <c r="C60" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D60" s="5" t="inlineStr">
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
         <is>
           <t>9801649305</t>
         </is>
       </c>
-      <c r="E60" s="6" t="n">
+      <c r="E60" s="2" t="n">
         <v>-65740358</v>
       </c>
-      <c r="F60" s="5" t="inlineStr">
+      <c r="F60" s="6" t="inlineStr">
         <is>
           <t>FACT PROVEEDOR</t>
         </is>
       </c>
-      <c r="G60" s="5" t="inlineStr">
+      <c r="G60" s="6" t="inlineStr">
         <is>
           <t>CSB</t>
         </is>
       </c>
-      <c r="H60" s="6" t="n">
+      <c r="H60" s="2" t="n">
         <v>-65740358</v>
       </c>
       <c r="I60" s="7" t="inlineStr">
@@ -1763,30 +1877,30 @@
       </c>
     </row>
     <row r="61">
-      <c r="C61" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D61" s="5" t="inlineStr">
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
         <is>
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E61" s="6" t="n">
+      <c r="E61" s="2" t="n">
         <v>-2</v>
       </c>
-      <c r="F61" s="5" t="inlineStr">
+      <c r="F61" s="6" t="inlineStr">
         <is>
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G61" s="5" t="inlineStr">
+      <c r="G61" s="6" t="inlineStr">
         <is>
           <t>551</t>
         </is>
       </c>
-      <c r="H61" s="6" t="n">
+      <c r="H61" s="2" t="n">
         <v>-2</v>
       </c>
       <c r="I61" s="7" t="inlineStr">
@@ -1796,30 +1910,30 @@
       </c>
     </row>
     <row r="62">
-      <c r="C62" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D62" s="5" t="inlineStr">
+      <c r="C62" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D62" s="6" t="inlineStr">
         <is>
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E62" s="6" t="n">
+      <c r="E62" s="2" t="n">
         <v>-143069</v>
       </c>
-      <c r="F62" s="5" t="inlineStr">
+      <c r="F62" s="6" t="inlineStr">
         <is>
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G62" s="5" t="inlineStr">
+      <c r="G62" s="6" t="inlineStr">
         <is>
           <t>551</t>
         </is>
       </c>
-      <c r="H62" s="6" t="n">
+      <c r="H62" s="2" t="n">
         <v>-143069</v>
       </c>
       <c r="I62" s="7" t="inlineStr">
@@ -1829,30 +1943,30 @@
       </c>
     </row>
     <row r="63">
-      <c r="C63" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D63" s="5" t="inlineStr">
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
         <is>
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E63" s="6" t="n">
+      <c r="E63" s="2" t="n">
         <v>-9553281</v>
       </c>
-      <c r="F63" s="5" t="inlineStr">
+      <c r="F63" s="6" t="inlineStr">
         <is>
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G63" s="5" t="inlineStr">
+      <c r="G63" s="6" t="inlineStr">
         <is>
           <t>551</t>
         </is>
       </c>
-      <c r="H63" s="6" t="n">
+      <c r="H63" s="2" t="n">
         <v>-9553281</v>
       </c>
       <c r="I63" s="7" t="inlineStr">
@@ -1862,30 +1976,30 @@
       </c>
     </row>
     <row r="64">
-      <c r="C64" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D64" s="5" t="inlineStr">
+      <c r="C64" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D64" s="6" t="inlineStr">
         <is>
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E64" s="6" t="n">
+      <c r="E64" s="2" t="n">
         <v>-97382</v>
       </c>
-      <c r="F64" s="5" t="inlineStr">
+      <c r="F64" s="6" t="inlineStr">
         <is>
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G64" s="5" t="inlineStr">
+      <c r="G64" s="6" t="inlineStr">
         <is>
           <t>551</t>
         </is>
       </c>
-      <c r="H64" s="6" t="n">
+      <c r="H64" s="2" t="n">
         <v>-97382</v>
       </c>
       <c r="I64" s="7" t="inlineStr">
@@ -1895,30 +2009,30 @@
       </c>
     </row>
     <row r="65">
-      <c r="C65" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D65" s="5" t="inlineStr">
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
         <is>
           <t>PMP1243639</t>
         </is>
       </c>
-      <c r="E65" s="6" t="n">
+      <c r="E65" s="2" t="n">
         <v>-649</v>
       </c>
-      <c r="F65" s="5" t="inlineStr">
+      <c r="F65" s="6" t="inlineStr">
         <is>
           <t>RECHAZO</t>
         </is>
       </c>
-      <c r="G65" s="5" t="inlineStr">
+      <c r="G65" s="6" t="inlineStr">
         <is>
           <t>551</t>
         </is>
       </c>
-      <c r="H65" s="6" t="n">
+      <c r="H65" s="2" t="n">
         <v>-649</v>
       </c>
       <c r="I65" s="7" t="inlineStr">
@@ -1928,30 +2042,30 @@
       </c>
     </row>
     <row r="66">
-      <c r="C66" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D66" s="5" t="inlineStr">
+      <c r="C66" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D66" s="6" t="inlineStr">
         <is>
           <t>PMP1243434</t>
         </is>
       </c>
-      <c r="E66" s="6" t="n">
+      <c r="E66" s="2" t="n">
         <v>38.15999999642372</v>
       </c>
-      <c r="F66" s="5" t="inlineStr">
+      <c r="F66" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G66" s="5" t="inlineStr">
+      <c r="G66" s="6" t="inlineStr">
         <is>
           <t>384</t>
         </is>
       </c>
-      <c r="H66" s="6" t="n">
+      <c r="H66" s="2" t="n">
         <v>38.15999999642372</v>
       </c>
       <c r="I66" s="7" t="inlineStr">
@@ -1961,30 +2075,30 @@
       </c>
     </row>
     <row r="67">
-      <c r="C67" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D67" s="5" t="inlineStr">
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
         <is>
           <t>PMP1243435</t>
         </is>
       </c>
-      <c r="E67" s="6" t="n">
+      <c r="E67" s="2" t="n">
         <v>-0.2399999983608723</v>
       </c>
-      <c r="F67" s="5" t="inlineStr">
+      <c r="F67" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G67" s="5" t="inlineStr">
+      <c r="G67" s="6" t="inlineStr">
         <is>
           <t>WOB</t>
         </is>
       </c>
-      <c r="H67" s="6" t="n">
+      <c r="H67" s="2" t="n">
         <v>-0.2399999983608723</v>
       </c>
       <c r="I67" s="7" t="inlineStr">
@@ -1994,30 +2108,30 @@
       </c>
     </row>
     <row r="68">
-      <c r="C68" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D68" s="5" t="inlineStr">
+      <c r="C68" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D68" s="6" t="inlineStr">
         <is>
           <t>PMP1243437</t>
         </is>
       </c>
-      <c r="E68" s="6" t="n">
+      <c r="E68" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="F68" s="5" t="inlineStr">
+      <c r="F68" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G68" s="5" t="inlineStr">
+      <c r="G68" s="6" t="inlineStr">
         <is>
           <t>384</t>
         </is>
       </c>
-      <c r="H68" s="6" t="n">
+      <c r="H68" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="I68" s="7" t="inlineStr">
@@ -2027,30 +2141,30 @@
       </c>
     </row>
     <row r="69">
-      <c r="C69" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D69" s="5" t="inlineStr">
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
         <is>
           <t>PMP1243438</t>
         </is>
       </c>
-      <c r="E69" s="6" t="n">
+      <c r="E69" s="2" t="n">
         <v>0.2800000011920929</v>
       </c>
-      <c r="F69" s="5" t="inlineStr">
+      <c r="F69" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G69" s="5" t="inlineStr">
+      <c r="G69" s="6" t="inlineStr">
         <is>
           <t>384</t>
         </is>
       </c>
-      <c r="H69" s="6" t="n">
+      <c r="H69" s="2" t="n">
         <v>0.2800000011920929</v>
       </c>
       <c r="I69" s="7" t="inlineStr">
@@ -2060,30 +2174,30 @@
       </c>
     </row>
     <row r="70">
-      <c r="C70" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D70" s="5" t="inlineStr">
+      <c r="C70" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D70" s="6" t="inlineStr">
         <is>
           <t>PMP1243439</t>
         </is>
       </c>
-      <c r="E70" s="6" t="n">
+      <c r="E70" s="2" t="n">
         <v>-0.2200000286102295</v>
       </c>
-      <c r="F70" s="5" t="inlineStr">
+      <c r="F70" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G70" s="5" t="inlineStr">
+      <c r="G70" s="6" t="inlineStr">
         <is>
           <t>WOB</t>
         </is>
       </c>
-      <c r="H70" s="6" t="n">
+      <c r="H70" s="2" t="n">
         <v>-0.2200000286102295</v>
       </c>
       <c r="I70" s="7" t="inlineStr">
@@ -2093,30 +2207,30 @@
       </c>
     </row>
     <row r="71">
-      <c r="C71" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D71" s="5" t="inlineStr">
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
         <is>
           <t>PMP1243546</t>
         </is>
       </c>
-      <c r="E71" s="6" t="n">
+      <c r="E71" s="2" t="n">
         <v>-1.700000002980232</v>
       </c>
-      <c r="F71" s="5" t="inlineStr">
+      <c r="F71" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G71" s="5" t="inlineStr">
+      <c r="G71" s="6" t="inlineStr">
         <is>
           <t>WOB</t>
         </is>
       </c>
-      <c r="H71" s="6" t="n">
+      <c r="H71" s="2" t="n">
         <v>-1.700000002980232</v>
       </c>
       <c r="I71" s="7" t="inlineStr">
@@ -2126,30 +2240,30 @@
       </c>
     </row>
     <row r="72">
-      <c r="C72" s="5" t="inlineStr">
-        <is>
-          <t>Descuentos no asociados a FC</t>
-        </is>
-      </c>
-      <c r="D72" s="5" t="inlineStr">
+      <c r="C72" s="6" t="inlineStr">
+        <is>
+          <t>Descuentos no asociados a FC</t>
+        </is>
+      </c>
+      <c r="D72" s="6" t="inlineStr">
         <is>
           <t>PMP1243639</t>
         </is>
       </c>
-      <c r="E72" s="6" t="n">
+      <c r="E72" s="2" t="n">
         <v>0.9399999976158142</v>
       </c>
-      <c r="F72" s="5" t="inlineStr">
+      <c r="F72" s="6" t="inlineStr">
         <is>
           <t>MENORES VALORES</t>
         </is>
       </c>
-      <c r="G72" s="5" t="inlineStr">
+      <c r="G72" s="6" t="inlineStr">
         <is>
           <t>384</t>
         </is>
       </c>
-      <c r="H72" s="6" t="n">
+      <c r="H72" s="2" t="n">
         <v>0.9399999976158142</v>
       </c>
       <c r="I72" s="7" t="inlineStr">

</xml_diff>